<commit_message>
updated with tests, new code (lstm)
</commit_message>
<xml_diff>
--- a/output/acción contra el hambre.xlsx
+++ b/output/acción contra el hambre.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>Pais-Año</t>
   </si>
@@ -22,25 +22,25 @@
     <t>ONU</t>
   </si>
   <si>
-    <t>Gross_National_Income</t>
+    <t>GDP</t>
   </si>
   <si>
     <t>Public_Grant</t>
   </si>
   <si>
-    <t>NGO_Country_Budget_Previous_Year</t>
-  </si>
-  <si>
-    <t>Vision_ONGD_LatinAmerica</t>
-  </si>
-  <si>
-    <t>Vision_ONGD_Africa</t>
-  </si>
-  <si>
-    <t>Vision_ONGD_Confessional</t>
-  </si>
-  <si>
-    <t>Vision_ONGD_Universal</t>
+    <t>Budget_Previous_Year</t>
+  </si>
+  <si>
+    <t>LatinAmerica</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Confessional</t>
+  </si>
+  <si>
+    <t>Universal</t>
   </si>
   <si>
     <t>Public_Funds_MAE</t>
@@ -109,16 +109,16 @@
     <t>Voluntarios_Extranjero</t>
   </si>
   <si>
-    <t>Total_subvencion_en_el_Pais_y_Anyo</t>
-  </si>
-  <si>
-    <t>Total_Fondos</t>
-  </si>
-  <si>
-    <t>Proporcion_Fondos_Privados</t>
-  </si>
-  <si>
-    <t>Proporcion_Fondos_MAE</t>
+    <t>Donor_Aid_Budget</t>
+  </si>
+  <si>
+    <t>Total_Funds</t>
+  </si>
+  <si>
+    <t>%_Private_Funds</t>
+  </si>
+  <si>
+    <t>%_MAE_Funds</t>
   </si>
   <si>
     <t>Anyo_ONG</t>
@@ -130,7 +130,7 @@
     <t>Colony</t>
   </si>
   <si>
-    <t>Delegacion</t>
+    <t>Delegation</t>
   </si>
   <si>
     <t>Visitado</t>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>2009_siria</t>
-  </si>
-  <si>
-    <t>..</t>
   </si>
   <si>
     <t>2009_palestina</t>
@@ -1018,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2620</v>
+        <v>2870.311589353206</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1140,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1380</v>
+        <v>1460.056109840828</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1262,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1620</v>
+        <v>1909.084588129339</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1384,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5130</v>
+        <v>6128.19547247793</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1506,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>3450</v>
+        <v>3972.630273980753</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1628,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>3970</v>
+        <v>4729.735976516416</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1750,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>2260</v>
+        <v>2100.656463590606</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1872,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>6880</v>
+        <v>7397.509860835168</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1993,8 +1990,8 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
-        <v>50</v>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2110,7 +2107,7 @@
     </row>
     <row r="11" spans="1:41">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2232,13 +2229,13 @@
     </row>
     <row r="12" spans="1:41">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>3240</v>
+        <v>3587.883798243964</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2354,13 +2351,13 @@
     </row>
     <row r="13" spans="1:41">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>3460</v>
+        <v>4168.505177067188</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2476,13 +2473,13 @@
     </row>
     <row r="14" spans="1:41">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>650</v>
+        <v>672.4244025624427</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2598,13 +2595,13 @@
     </row>
     <row r="15" spans="1:41">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>690</v>
+        <v>710.2742021758368</v>
       </c>
       <c r="D15">
         <v>2000000</v>
@@ -2720,13 +2717,13 @@
     </row>
     <row r="16" spans="1:41">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1170</v>
+        <v>1610.923908476106</v>
       </c>
       <c r="D16">
         <v>2000000</v>
@@ -2842,13 +2839,13 @@
     </row>
     <row r="17" spans="1:41">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>350</v>
+        <v>473.2998774917226</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2964,13 +2961,13 @@
     </row>
     <row r="18" spans="1:41">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1340</v>
+        <v>1280.225469721551</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3086,13 +3083,13 @@
     </row>
     <row r="19" spans="1:41">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>2710</v>
+        <v>2898.942214704482</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -3208,13 +3205,13 @@
     </row>
     <row r="20" spans="1:41">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>1460</v>
+        <v>1503.870423231357</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -3330,13 +3327,13 @@
     </row>
     <row r="21" spans="1:41">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>1780</v>
+        <v>1955.461557360978</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -3452,13 +3449,13 @@
     </row>
     <row r="22" spans="1:41">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>5610</v>
+        <v>6336.709213679884</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3574,13 +3571,13 @@
     </row>
     <row r="23" spans="1:41">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>4390</v>
+        <v>4633.590358399045</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -3696,13 +3693,13 @@
     </row>
     <row r="24" spans="1:41">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>4070</v>
+        <v>4355.934938677345</v>
       </c>
       <c r="D24">
         <v>2500000</v>
@@ -3818,13 +3815,13 @@
     </row>
     <row r="25" spans="1:41">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>4410</v>
+        <v>5082.354756663512</v>
       </c>
       <c r="D25">
         <v>2500000</v>
@@ -3940,13 +3937,13 @@
     </row>
     <row r="26" spans="1:41">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2460</v>
+        <v>2217.474008566157</v>
       </c>
       <c r="D26">
         <v>3200000</v>
@@ -4062,13 +4059,13 @@
     </row>
     <row r="27" spans="1:41">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>7480</v>
+        <v>7761.646190572197</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4184,13 +4181,13 @@
     </row>
     <row r="28" spans="1:41">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28" t="s">
-        <v>50</v>
+      <c r="C28">
+        <v>0</v>
       </c>
       <c r="D28">
         <v>2000000</v>
@@ -4306,7 +4303,7 @@
     </row>
     <row r="29" spans="1:41">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4428,13 +4425,13 @@
     </row>
     <row r="30" spans="1:41">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>4080</v>
+        <v>4233.575210230672</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4550,13 +4547,13 @@
     </row>
     <row r="31" spans="1:41">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>4690</v>
+        <v>4539.002521388361</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -4672,13 +4669,13 @@
     </row>
     <row r="32" spans="1:41">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>3990</v>
+        <v>4022.237688257</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -4794,13 +4791,13 @@
     </row>
     <row r="33" spans="1:41">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>650</v>
+        <v>694.6031345426339</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -4916,13 +4913,13 @@
     </row>
     <row r="34" spans="1:41">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34">
-        <v>730</v>
+        <v>711.1128122770988</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -5038,13 +5035,13 @@
     </row>
     <row r="35" spans="1:41">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35">
-        <v>1240</v>
+        <v>1629.435089125503</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -5160,13 +5157,13 @@
     </row>
     <row r="36" spans="1:41">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36">
-        <v>360</v>
+        <v>466.0709276378625</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -5282,13 +5279,13 @@
     </row>
     <row r="37" spans="1:41">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37">
-        <v>2860</v>
+        <v>2965.153206179127</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -5404,13 +5401,13 @@
     </row>
     <row r="38" spans="1:41">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>1570</v>
+        <v>1577.487171555845</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -5526,13 +5523,13 @@
     </row>
     <row r="39" spans="1:41">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>1990</v>
+        <v>2024.117324382548</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -5648,13 +5645,13 @@
     </row>
     <row r="40" spans="1:41">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>6320</v>
+        <v>6711.616186806423</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -5770,13 +5767,13 @@
     </row>
     <row r="41" spans="1:41">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>4870</v>
+        <v>4921.848409120176</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -5892,13 +5889,13 @@
     </row>
     <row r="42" spans="1:41">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>4480</v>
+        <v>4479.398934239905</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -6014,13 +6011,13 @@
     </row>
     <row r="43" spans="1:41">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>4970</v>
+        <v>5360.226632400601</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -6136,13 +6133,13 @@
     </row>
     <row r="44" spans="1:41">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>2610</v>
+        <v>2264.394087033834</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -6258,13 +6255,13 @@
     </row>
     <row r="45" spans="1:41">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>3400</v>
+        <v>3500.527492856126</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -6380,13 +6377,13 @@
     </row>
     <row r="46" spans="1:41">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>11230</v>
+        <v>11678.13078702468</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -6502,13 +6499,13 @@
     </row>
     <row r="47" spans="1:41">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>7580</v>
+        <v>7453.823475007535</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -6624,13 +6621,13 @@
     </row>
     <row r="48" spans="1:41">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
-      <c r="C48" t="s">
-        <v>50</v>
+      <c r="C48">
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -6746,7 +6743,7 @@
     </row>
     <row r="49" spans="1:41">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -6868,13 +6865,13 @@
     </row>
     <row r="50" spans="1:41">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>3100</v>
+        <v>2999.422762626143</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -6990,13 +6987,13 @@
     </row>
     <row r="51" spans="1:41">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>1690</v>
+        <v>1657.651524528445</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -7112,13 +7109,13 @@
     </row>
     <row r="52" spans="1:41">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>2250</v>
+        <v>2094.024217383061</v>
       </c>
       <c r="D52">
         <v>478380</v>
@@ -7234,13 +7231,13 @@
     </row>
     <row r="53" spans="1:41">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>4760</v>
+        <v>4394.543881413723</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -7356,13 +7353,13 @@
     </row>
     <row r="54" spans="1:41">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>7290</v>
+        <v>6911.59200404802</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -7478,13 +7475,13 @@
     </row>
     <row r="55" spans="1:41">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>5790</v>
+        <v>5642.578115155247</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -7600,13 +7597,13 @@
     </row>
     <row r="56" spans="1:41">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>2970</v>
+        <v>2379.668184479739</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -7722,13 +7719,13 @@
     </row>
     <row r="57" spans="1:41">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>3970</v>
+        <v>3751.003475853037</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -7844,13 +7841,13 @@
     </row>
     <row r="58" spans="1:41">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>7590</v>
+        <v>7179.116970062444</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -7966,13 +7963,13 @@
     </row>
     <row r="59" spans="1:41">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
-      <c r="C59" t="s">
-        <v>50</v>
+      <c r="C59">
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -8088,7 +8085,7 @@
     </row>
     <row r="60" spans="1:41">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -8210,13 +8207,13 @@
     </row>
     <row r="61" spans="1:41">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>670</v>
+        <v>719.6981727039259</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -8332,13 +8329,13 @@
     </row>
     <row r="62" spans="1:41">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62">
-        <v>730</v>
+        <v>684.6474015015979</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -8454,13 +8451,13 @@
     </row>
     <row r="63" spans="1:41">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63">
-        <v>1360</v>
+        <v>1652.714170143609</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -8576,13 +8573,13 @@
     </row>
     <row r="64" spans="1:41">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64">
-        <v>380</v>
+        <v>495.763971160512</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -8698,13 +8695,13 @@
     </row>
     <row r="65" spans="1:41">
       <c r="A65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65">
-        <v>1330</v>
+        <v>1291.622214254295</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -8820,13 +8817,13 @@
     </row>
     <row r="66" spans="1:41">
       <c r="A66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66">
-        <v>2840</v>
+        <v>2634.85005236495</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -8942,13 +8939,13 @@
     </row>
     <row r="67" spans="1:41">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>12740</v>
+        <v>12876.88928835506</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -9050,7 +9047,7 @@
         <v>1</v>
       </c>
       <c r="AL67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM67">
         <v>0</v>
@@ -9064,13 +9061,13 @@
     </row>
     <row r="68" spans="1:41">
       <c r="A68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>3320</v>
+        <v>3056.152683606517</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -9186,13 +9183,13 @@
     </row>
     <row r="69" spans="1:41">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>1780</v>
+        <v>1716.389195271215</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -9308,13 +9305,13 @@
     </row>
     <row r="70" spans="1:41">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>2590</v>
+        <v>2201.396847776877</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -9430,13 +9427,13 @@
     </row>
     <row r="71" spans="1:41">
       <c r="A71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>5510</v>
+        <v>4699.493713911862</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -9552,13 +9549,13 @@
     </row>
     <row r="72" spans="1:41">
       <c r="A72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="C72">
-        <v>7910</v>
+        <v>7200.731056811853</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -9674,13 +9671,13 @@
     </row>
     <row r="73" spans="1:41">
       <c r="A73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>6420</v>
+        <v>5919.20956823756</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -9796,13 +9793,13 @@
     </row>
     <row r="74" spans="1:41">
       <c r="A74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>3290</v>
+        <v>2497.68592515536</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -9918,13 +9915,13 @@
     </row>
     <row r="75" spans="1:41">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>4300</v>
+        <v>3898.554689331348</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -10040,13 +10037,13 @@
     </row>
     <row r="76" spans="1:41">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76">
-        <v>7610</v>
+        <v>6978.952586250825</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -10162,13 +10159,13 @@
     </row>
     <row r="77" spans="1:41">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
-      <c r="C77" t="s">
-        <v>50</v>
+      <c r="C77">
+        <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -10284,7 +10281,7 @@
     </row>
     <row r="78" spans="1:41">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -10406,13 +10403,13 @@
     </row>
     <row r="79" spans="1:41">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79">
-        <v>700</v>
+        <v>731.5588677998553</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -10528,13 +10525,13 @@
     </row>
     <row r="80" spans="1:41">
       <c r="A80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80">
-        <v>780</v>
+        <v>680.3923729568069</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -10650,13 +10647,13 @@
     </row>
     <row r="81" spans="1:41">
       <c r="A81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81">
-        <v>1450</v>
+        <v>1671.292192516047</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -10772,13 +10769,13 @@
     </row>
     <row r="82" spans="1:41">
       <c r="A82" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82">
-        <v>400</v>
+        <v>503.3023574516347</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -10894,13 +10891,13 @@
     </row>
     <row r="83" spans="1:41">
       <c r="A83" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83">
-        <v>1360</v>
+        <v>1291.415042301529</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -11016,13 +11013,13 @@
     </row>
     <row r="84" spans="1:41">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84">
-        <v>3030</v>
+        <v>2632.058233068435</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -11138,13 +11135,13 @@
     </row>
     <row r="85" spans="1:41">
       <c r="A85" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="C85">
-        <v>12640</v>
+        <v>12644.6890235017</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -11246,7 +11243,7 @@
         <v>1</v>
       </c>
       <c r="AL85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM85">
         <v>0</v>
@@ -11260,13 +11257,13 @@
     </row>
     <row r="86" spans="1:41">
       <c r="A86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86">
-        <v>2830</v>
+        <v>2286.013198234259</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -11382,13 +11379,13 @@
     </row>
     <row r="87" spans="1:41">
       <c r="A87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>8190</v>
+        <v>7449.08671983612</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -11504,13 +11501,13 @@
     </row>
     <row r="88" spans="1:41">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88">
-        <v>3230</v>
+        <v>2648.294169302945</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -11626,13 +11623,13 @@
     </row>
     <row r="89" spans="1:41">
       <c r="A89" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B89">
         <v>0</v>
       </c>
       <c r="C89">
-        <v>3450</v>
+        <v>2612.856880840196</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -11748,13 +11745,13 @@
     </row>
     <row r="90" spans="1:41">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>4500</v>
+        <v>4069.424500171965</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -11870,13 +11867,13 @@
     </row>
     <row r="91" spans="1:41">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>3460</v>
+        <v>3137.260298393558</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -11992,13 +11989,13 @@
     </row>
     <row r="92" spans="1:41">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>740</v>
+        <v>741.0381351906716</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -12114,13 +12111,13 @@
     </row>
     <row r="93" spans="1:41">
       <c r="A93" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="C93">
-        <v>7500</v>
+        <v>6753.607115829548</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -12236,13 +12233,13 @@
     </row>
     <row r="94" spans="1:41">
       <c r="A94" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94">
-        <v>810</v>
+        <v>707.8672001573369</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -12358,13 +12355,13 @@
     </row>
     <row r="95" spans="1:41">
       <c r="A95" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95">
-        <v>1390</v>
+        <v>1692.460946584157</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -12480,13 +12477,13 @@
     </row>
     <row r="96" spans="1:41">
       <c r="A96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B96">
         <v>1</v>
       </c>
       <c r="C96">
-        <v>410</v>
+        <v>515.8271637832048</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -12602,13 +12599,13 @@
     </row>
     <row r="97" spans="1:41">
       <c r="A97" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97">
-        <v>6530</v>
+        <v>5996.49696468919</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -12724,13 +12721,13 @@
     </row>
     <row r="98" spans="1:41">
       <c r="A98" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98">
-        <v>1380</v>
+        <v>1338.716747746975</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -12846,13 +12843,13 @@
     </row>
     <row r="99" spans="1:41">
       <c r="A99" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
-      <c r="C99" t="s">
-        <v>50</v>
+      <c r="C99">
+        <v>0</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -12968,13 +12965,13 @@
     </row>
     <row r="100" spans="1:41">
       <c r="A100" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100">
-        <v>12560</v>
+        <v>13277.7607681612</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -13090,13 +13087,13 @@
     </row>
     <row r="101" spans="1:41">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>2960</v>
+        <v>2361.056581219794</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -13212,13 +13209,13 @@
     </row>
     <row r="102" spans="1:41">
       <c r="A102" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="C102">
-        <v>7330</v>
+        <v>7580.275568826287</v>
       </c>
       <c r="D102">
         <v>129199</v>
@@ -13334,13 +13331,13 @@
     </row>
     <row r="103" spans="1:41">
       <c r="A103" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>3360</v>
+        <v>2703.742092148914</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -13456,13 +13453,13 @@
     </row>
     <row r="104" spans="1:41">
       <c r="A104" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="C104">
-        <v>3510</v>
+        <v>2735.187532014817</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -13578,13 +13575,13 @@
     </row>
     <row r="105" spans="1:41">
       <c r="A105" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>4110</v>
+        <v>4185.813876020487</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -13700,13 +13697,13 @@
     </row>
     <row r="106" spans="1:41">
       <c r="A106" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>3620</v>
+        <v>3210.869677115934</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -13822,13 +13819,13 @@
     </row>
     <row r="107" spans="1:41">
       <c r="A107" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>750</v>
+        <v>750.4706590411453</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -13944,13 +13941,13 @@
     </row>
     <row r="108" spans="1:41">
       <c r="A108" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="C108">
-        <v>7290</v>
+        <v>6487.899081675427</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -14066,13 +14063,13 @@
     </row>
     <row r="109" spans="1:41">
       <c r="A109" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>790</v>
+        <v>729.7808175407341</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -14188,13 +14185,13 @@
     </row>
     <row r="110" spans="1:41">
       <c r="A110" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="C110">
-        <v>1270</v>
+        <v>1732.587316450496</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -14310,13 +14307,13 @@
     </row>
     <row r="111" spans="1:41">
       <c r="A111" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="C111">
-        <v>390</v>
+        <v>517.8609592583078</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -14432,13 +14429,13 @@
     </row>
     <row r="112" spans="1:41">
       <c r="A112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>6340</v>
+        <v>6114.227214287786</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -14554,13 +14551,13 @@
     </row>
     <row r="113" spans="1:41">
       <c r="A113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="C113">
-        <v>1320</v>
+        <v>1384.519227335143</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -14676,13 +14673,13 @@
     </row>
     <row r="114" spans="1:41">
       <c r="A114" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
-      <c r="C114" t="s">
-        <v>50</v>
+      <c r="C114">
+        <v>0</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -14798,13 +14795,13 @@
     </row>
     <row r="115" spans="1:41">
       <c r="A115" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>11960</v>
+        <v>13853.0971344428</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -14920,13 +14917,13 @@
     </row>
     <row r="116" spans="1:41">
       <c r="A116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="C116">
-        <v>3040</v>
+        <v>2425.561644739583</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -15042,13 +15039,13 @@
     </row>
     <row r="117" spans="1:41">
       <c r="A117" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>6460</v>
+        <v>7633.969039669125</v>
       </c>
       <c r="D117">
         <v>129199</v>
@@ -15164,13 +15161,13 @@
     </row>
     <row r="118" spans="1:41">
       <c r="A118" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>5810</v>
+        <v>5176.058803160127</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -15286,13 +15283,13 @@
     </row>
     <row r="119" spans="1:41">
       <c r="A119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119">
-        <v>3460</v>
+        <v>2761.386198249428</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -15408,13 +15405,13 @@
     </row>
     <row r="120" spans="1:41">
       <c r="A120" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120">
-        <v>3570</v>
+        <v>2886.897484630703</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -15530,13 +15527,13 @@
     </row>
     <row r="121" spans="1:41">
       <c r="A121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>3830</v>
+        <v>4304.896180977176</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -15652,13 +15649,13 @@
     </row>
     <row r="122" spans="1:41">
       <c r="A122" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122">
-        <v>3800</v>
+        <v>3242.636921959078</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -15774,13 +15771,13 @@
     </row>
     <row r="123" spans="1:41">
       <c r="A123" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>770</v>
+        <v>809.9545825255682</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -15896,13 +15893,13 @@
     </row>
     <row r="124" spans="1:41">
       <c r="A124" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>7250</v>
+        <v>6411.986543373589</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -16018,13 +16015,13 @@
     </row>
     <row r="125" spans="1:41">
       <c r="A125" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B125">
         <v>1</v>
       </c>
       <c r="C125">
-        <v>780</v>
+        <v>749.2194349876407</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -16140,13 +16137,13 @@
     </row>
     <row r="126" spans="1:41">
       <c r="A126" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B126">
         <v>1</v>
       </c>
       <c r="C126">
-        <v>1160</v>
+        <v>1705.033923663474</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -16262,13 +16259,13 @@
     </row>
     <row r="127" spans="1:41">
       <c r="A127" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
       <c r="C127">
-        <v>2000</v>
+        <v>1895.214690888655</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -16384,13 +16381,13 @@
     </row>
     <row r="128" spans="1:41">
       <c r="A128" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B128">
         <v>1</v>
       </c>
       <c r="C128">
-        <v>370</v>
+        <v>526.5953412037009</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -16506,13 +16503,13 @@
     </row>
     <row r="129" spans="1:41">
       <c r="A129" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B129">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>6120</v>
+        <v>6262.368904654469</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -16628,13 +16625,13 @@
     </row>
     <row r="130" spans="1:41">
       <c r="A130" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B130">
         <v>1</v>
       </c>
       <c r="C130">
-        <v>1270</v>
+        <v>1431.756130822538</v>
       </c>
       <c r="D130">
         <v>398000</v>
@@ -16750,13 +16747,13 @@
     </row>
     <row r="131" spans="1:41">
       <c r="A131" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
-      <c r="C131" t="s">
-        <v>50</v>
+      <c r="C131">
+        <v>0</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -16872,7 +16869,7 @@
     </row>
     <row r="132" spans="1:41">
       <c r="A132" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -16994,13 +16991,13 @@
     </row>
     <row r="133" spans="1:41">
       <c r="A133" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>11180</v>
+        <v>14062.73378768283</v>
       </c>
       <c r="D133">
         <v>0</v>

</xml_diff>